<commit_message>
- Add excel file containing preloaded options - Change default ER DC contribution rate in input file
</commit_message>
<xml_diff>
--- a/NDPERS Funding Model Inputs.xlsx
+++ b/NDPERS Funding Model Inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/truongbui/Dropbox/Work/Reason/Reason Work/R projects/Plan Models/North Dakota PERS/NDPERS-Funding Model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1611B995-1FD8-D74B-9967-626EF0D44EAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF1A02D-E54C-E241-B516-0C0E9898C186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1985,7 +1985,7 @@
   <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2145,8 +2145,8 @@
       <c r="B15" t="s">
         <v>189</v>
       </c>
-      <c r="C15" s="28">
-        <v>7.0000000000000007E-2</v>
+      <c r="C15" s="15">
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update lower DR, add custom return input, and add more cash infusion inputs
</commit_message>
<xml_diff>
--- a/NDPERS Funding Model Inputs.xlsx
+++ b/NDPERS Funding Model Inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/truongbui/Dropbox/Work/Reason/Reason Work/R projects/Plan Models/North Dakota PERS/NDPERS-Funding Model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF1A02D-E54C-E241-B516-0C0E9898C186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BDFD2FF-6A60-E84F-B15E-6929ED34CE12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Numeric Inputs" sheetId="1" r:id="rId1"/>
@@ -324,7 +324,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="310">
   <si>
     <t>Economic Inputs</t>
   </si>
@@ -1064,21 +1064,6 @@
     <t>Supplemental</t>
   </si>
   <si>
-    <t>Bill 1 - Additional ER contribution rate</t>
-  </si>
-  <si>
-    <t>Bill 1 - Additional cash infusion (2021)</t>
-  </si>
-  <si>
-    <t>Bill 2 - Legacy Fund transfer - % of earnings transferred to GF</t>
-  </si>
-  <si>
-    <t>Bill 2 - Legacy Fund transfer - % of earnings transferred to PERS</t>
-  </si>
-  <si>
-    <t>Bill 2 - Legacy Fund transfer - funded level threshold</t>
-  </si>
-  <si>
     <t>Transfers</t>
   </si>
   <si>
@@ -1233,6 +1218,42 @@
   </si>
   <si>
     <t>NewHirePayroll</t>
+  </si>
+  <si>
+    <t>Annual Cash Infusion</t>
+  </si>
+  <si>
+    <t>CashInfusion_Annual</t>
+  </si>
+  <si>
+    <t>Model Investment Return</t>
+  </si>
+  <si>
+    <t>model_return</t>
+  </si>
+  <si>
+    <t>Additional cash infusion (2021)</t>
+  </si>
+  <si>
+    <t>Legacy Fund transfer - % of earnings transferred to GF</t>
+  </si>
+  <si>
+    <t>Legacy Fund transfer - % of earnings transferred to PERS</t>
+  </si>
+  <si>
+    <t>Legacy Fund transfer - funded level threshold</t>
+  </si>
+  <si>
+    <t>Additional EE contribution rate</t>
+  </si>
+  <si>
+    <t>Additional ER contribution rate</t>
+  </si>
+  <si>
+    <t>ER_Additional_Rate</t>
+  </si>
+  <si>
+    <t>EE_Additional_Rate</t>
   </si>
 </sst>
 </file>
@@ -1467,7 +1488,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1628,6 +1649,7 @@
     <xf numFmtId="166" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1982,10 +2004,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2020,7 +2042,7 @@
         <v>177</v>
       </c>
       <c r="C3" s="27">
-        <v>7.0000000000000007E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2042,152 +2064,152 @@
         <v>179</v>
       </c>
       <c r="C5" s="27">
-        <v>7.0000000000000007E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>300</v>
+      </c>
+      <c r="B6" t="s">
+        <v>301</v>
+      </c>
+      <c r="C6" s="27">
+        <v>6.5000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C7" s="27">
         <v>2.2499999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="26" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="26" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>98</v>
-      </c>
-      <c r="B8" t="s">
-        <v>99</v>
-      </c>
-      <c r="C8" s="28">
-        <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>98</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C9">
-        <v>2021</v>
+        <v>99</v>
+      </c>
+      <c r="C9" s="28">
+        <v>0.5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>214</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>226</v>
-      </c>
-      <c r="C10" s="15">
-        <v>0.10979999999999999</v>
+        <v>62</v>
+      </c>
+      <c r="C10">
+        <v>2021</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B11" t="s">
-        <v>175</v>
-      </c>
-      <c r="C11" s="76">
-        <v>9.7918409999999997E-2</v>
+        <v>226</v>
+      </c>
+      <c r="C11" s="15">
+        <v>0.10979999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>215</v>
       </c>
       <c r="B12" t="s">
-        <v>180</v>
-      </c>
-      <c r="C12" s="27">
-        <v>0</v>
+        <v>175</v>
+      </c>
+      <c r="C12" s="76">
+        <v>9.7918409999999997E-2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>191</v>
+        <v>57</v>
       </c>
       <c r="B13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C13" s="37">
-        <v>0.5</v>
+        <v>180</v>
+      </c>
+      <c r="C13" s="27">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>102</v>
+        <v>191</v>
       </c>
       <c r="B14" t="s">
-        <v>188</v>
-      </c>
-      <c r="C14" s="28">
-        <v>0</v>
+        <v>192</v>
+      </c>
+      <c r="C14" s="37">
+        <v>0.5</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B15" t="s">
-        <v>189</v>
-      </c>
-      <c r="C15" s="15">
-        <v>2.8000000000000001E-2</v>
+        <v>188</v>
+      </c>
+      <c r="C15" s="28">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>194</v>
+        <v>103</v>
       </c>
       <c r="B16" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="C16" s="15">
-        <v>2.75E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>218</v>
+        <v>194</v>
       </c>
       <c r="B17" t="s">
-        <v>220</v>
+        <v>195</v>
       </c>
       <c r="C17" s="15">
-        <v>1</v>
+        <v>2.75E-2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>218</v>
+      </c>
+      <c r="B18" t="s">
+        <v>220</v>
+      </c>
+      <c r="C18" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>219</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>221</v>
-      </c>
-      <c r="C18" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="53" t="s">
-        <v>239</v>
-      </c>
-      <c r="B19" t="s">
-        <v>242</v>
       </c>
       <c r="C19" s="15">
         <v>0</v>
@@ -2195,10 +2217,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="53" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B20" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C20" s="15">
         <v>0</v>
@@ -2206,568 +2228,601 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="53" t="s">
+        <v>240</v>
+      </c>
+      <c r="B21" t="s">
+        <v>243</v>
+      </c>
+      <c r="C21" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="53" t="s">
         <v>241</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>244</v>
       </c>
-      <c r="C21" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="69" t="s">
-        <v>293</v>
-      </c>
-      <c r="B22" t="s">
-        <v>295</v>
-      </c>
       <c r="C22" s="15">
-        <v>1.7500000000000002E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="64" t="s">
-        <v>292</v>
+      <c r="A23" s="69" t="s">
+        <v>288</v>
       </c>
       <c r="B23" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C23" s="15">
         <v>1.7500000000000002E-2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="26" t="s">
+      <c r="A24" s="64" t="s">
+        <v>287</v>
+      </c>
+      <c r="B24" t="s">
+        <v>289</v>
+      </c>
+      <c r="C24" s="15">
+        <v>1.7500000000000002E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="26" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>16</v>
-      </c>
-      <c r="B25" t="s">
-        <v>63</v>
-      </c>
-      <c r="C25" s="27">
-        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>105</v>
+        <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>106</v>
+        <v>63</v>
       </c>
       <c r="C26" s="27">
-        <v>2.5000000000000001E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>5</v>
+        <v>105</v>
       </c>
       <c r="B27" t="s">
-        <v>61</v>
+        <v>106</v>
       </c>
       <c r="C27" s="27">
-        <v>0</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>65</v>
-      </c>
-      <c r="C28">
-        <v>66</v>
+        <v>61</v>
+      </c>
+      <c r="C28" s="27">
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>107</v>
+        <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>109</v>
-      </c>
-      <c r="C29" s="27">
-        <v>2.3E-3</v>
+        <v>65</v>
+      </c>
+      <c r="C29">
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>261</v>
+        <v>107</v>
       </c>
       <c r="B30" t="s">
-        <v>262</v>
+        <v>109</v>
       </c>
       <c r="C30" s="27">
-        <v>4.3200000000000002E-2</v>
+        <v>2.3E-3</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>108</v>
+        <v>256</v>
       </c>
       <c r="B31" t="s">
-        <v>190</v>
-      </c>
-      <c r="C31" s="36">
-        <v>8.5</v>
+        <v>257</v>
+      </c>
+      <c r="C31" s="27">
+        <v>4.3200000000000002E-2</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>4</v>
+        <v>108</v>
       </c>
       <c r="B32" t="s">
-        <v>64</v>
-      </c>
-      <c r="C32" s="27">
-        <v>3.5000000000000003E-2</v>
+        <v>190</v>
+      </c>
+      <c r="C32" s="36">
+        <v>8.5</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" s="27">
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>216</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>217</v>
       </c>
-      <c r="C33" s="27">
+      <c r="C34" s="27">
         <v>0.98</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="26" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="26" t="s">
         <v>245</v>
       </c>
-      <c r="C34" s="27"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="54" t="s">
-        <v>246</v>
-      </c>
-      <c r="B35" t="s">
-        <v>209</v>
-      </c>
-      <c r="C35" s="55">
-        <v>0</v>
-      </c>
+      <c r="C35" s="27"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="54" t="s">
-        <v>247</v>
+        <v>307</v>
       </c>
       <c r="B36" t="s">
-        <v>277</v>
-      </c>
-      <c r="C36" s="56">
+        <v>308</v>
+      </c>
+      <c r="C36" s="55">
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="54" t="s">
-        <v>248</v>
+        <v>306</v>
       </c>
       <c r="B37" t="s">
-        <v>278</v>
-      </c>
-      <c r="C37" s="57">
+        <v>309</v>
+      </c>
+      <c r="C37" s="55">
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="54" t="s">
-        <v>249</v>
+        <v>302</v>
       </c>
       <c r="B38" t="s">
-        <v>279</v>
-      </c>
-      <c r="C38" s="55">
-        <v>0.14000000000000001</v>
+        <v>272</v>
+      </c>
+      <c r="C38" s="56">
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="54" t="s">
-        <v>250</v>
+        <v>298</v>
       </c>
       <c r="B39" t="s">
-        <v>280</v>
-      </c>
-      <c r="C39" s="55">
+        <v>299</v>
+      </c>
+      <c r="C39" s="56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="54" t="s">
+        <v>303</v>
+      </c>
+      <c r="B40" t="s">
+        <v>273</v>
+      </c>
+      <c r="C40" s="57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="54" t="s">
+        <v>304</v>
+      </c>
+      <c r="B41" t="s">
+        <v>274</v>
+      </c>
+      <c r="C41" s="55">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="54" t="s">
+        <v>305</v>
+      </c>
+      <c r="B42" t="s">
+        <v>275</v>
+      </c>
+      <c r="C42" s="55">
         <v>0.9</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="26" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C40" s="27"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="35" t="s">
+      <c r="C43" s="27"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="35" t="s">
         <v>157</v>
       </c>
-      <c r="B41" t="s">
-        <v>264</v>
-      </c>
-      <c r="C41" s="36">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="35" t="s">
+      <c r="B44" t="s">
+        <v>259</v>
+      </c>
+      <c r="C44" s="36">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="35" t="s">
         <v>158</v>
       </c>
-      <c r="B42" t="s">
-        <v>267</v>
-      </c>
-      <c r="C42" s="36">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="35" t="s">
-        <v>265</v>
-      </c>
-      <c r="B43" t="s">
-        <v>266</v>
-      </c>
-      <c r="C43" s="36">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>268</v>
-      </c>
-      <c r="B44" t="s">
-        <v>273</v>
-      </c>
-      <c r="C44" s="27">
-        <v>3.5000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>271</v>
-      </c>
       <c r="B45" t="s">
-        <v>274</v>
-      </c>
-      <c r="C45" s="15">
-        <v>3.5000000000000003E-2</v>
+        <v>262</v>
+      </c>
+      <c r="C45" s="36">
+        <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>120</v>
+      <c r="A46" s="35" t="s">
+        <v>260</v>
       </c>
       <c r="B46" t="s">
-        <v>121</v>
-      </c>
-      <c r="C46" s="27">
-        <v>99.99</v>
+        <v>261</v>
+      </c>
+      <c r="C46" s="36">
+        <v>20</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>210</v>
+        <v>263</v>
       </c>
       <c r="B47" t="s">
-        <v>237</v>
-      </c>
-      <c r="C47" s="63">
-        <v>7.0000000000000007E-2</v>
+        <v>268</v>
+      </c>
+      <c r="C47" s="27">
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>238</v>
+        <v>266</v>
       </c>
       <c r="B48" t="s">
-        <v>236</v>
-      </c>
-      <c r="C48" s="63">
-        <v>7.0000000000000007E-2</v>
+        <v>269</v>
+      </c>
+      <c r="C48" s="15">
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>211</v>
+        <v>120</v>
       </c>
       <c r="B49" t="s">
-        <v>213</v>
-      </c>
-      <c r="C49" s="63">
-        <v>7.2599999999999998E-2</v>
+        <v>121</v>
+      </c>
+      <c r="C49" s="27">
+        <v>99.99</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B50" t="s">
-        <v>110</v>
+        <v>237</v>
       </c>
       <c r="C50" s="63">
-        <v>8.2600000000000007E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>296</v>
+        <v>238</v>
       </c>
       <c r="B51" t="s">
-        <v>297</v>
-      </c>
-      <c r="C51" s="15">
-        <v>0.06</v>
+        <v>236</v>
+      </c>
+      <c r="C51" s="63">
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>12</v>
+        <v>211</v>
       </c>
       <c r="B52" t="s">
-        <v>68</v>
-      </c>
-      <c r="C52">
-        <v>0.8</v>
+        <v>213</v>
+      </c>
+      <c r="C52" s="63">
+        <v>7.2599999999999998E-2</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>13</v>
+        <v>212</v>
       </c>
       <c r="B53" t="s">
-        <v>69</v>
-      </c>
-      <c r="C53">
-        <v>1.2</v>
+        <v>110</v>
+      </c>
+      <c r="C53" s="63">
+        <v>8.2600000000000007E-2</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>19</v>
-      </c>
-      <c r="C54" s="27">
-        <f>D54-1%</f>
-        <v>6.2499999999999993E-2</v>
-      </c>
-      <c r="D54" s="27">
-        <v>7.2499999999999995E-2</v>
-      </c>
-      <c r="E54" s="27">
-        <f>D54+1%</f>
-        <v>8.249999999999999E-2</v>
+        <v>291</v>
+      </c>
+      <c r="B54" t="s">
+        <v>292</v>
+      </c>
+      <c r="C54" s="15">
+        <v>0.06</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>20</v>
-      </c>
-      <c r="C55" s="30">
-        <f>C56+C57</f>
-        <v>5270.3829970000006</v>
-      </c>
-      <c r="D55" s="30">
-        <f>D56+D57</f>
-        <v>4731.9598219999998</v>
-      </c>
-      <c r="E55" s="30">
-        <f>E56+E57</f>
-        <v>4282.6246919999994</v>
+        <v>12</v>
+      </c>
+      <c r="B55" t="s">
+        <v>68</v>
+      </c>
+      <c r="C55">
+        <v>0.8</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>21</v>
-      </c>
-      <c r="C56" s="30">
-        <f>D56</f>
-        <v>2057.857317</v>
-      </c>
-      <c r="D56" s="30">
-        <v>2057.857317</v>
-      </c>
-      <c r="E56" s="30">
-        <f>D56</f>
-        <v>2057.857317</v>
+        <v>13</v>
+      </c>
+      <c r="B56" t="s">
+        <v>69</v>
+      </c>
+      <c r="C56">
+        <v>1.2</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>22</v>
-      </c>
-      <c r="C57" s="30">
-        <v>3212.5256800000002</v>
-      </c>
-      <c r="D57" s="30">
-        <v>2674.1025049999998</v>
-      </c>
-      <c r="E57" s="30">
-        <v>2224.7673749999999</v>
+        <v>19</v>
+      </c>
+      <c r="C57" s="27">
+        <f>D57-1%</f>
+        <v>6.2499999999999993E-2</v>
+      </c>
+      <c r="D57" s="27">
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="E57" s="27">
+        <f>D57+1%</f>
+        <v>8.249999999999999E-2</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>23</v>
-      </c>
-      <c r="B58" t="s">
-        <v>70</v>
-      </c>
-      <c r="C58" s="29">
-        <f>((C55/E55)^(1/2)-1)*100</f>
-        <v>10.934359407830318</v>
+        <v>20</v>
+      </c>
+      <c r="C58" s="30">
+        <f>C59+C60</f>
+        <v>5270.3829970000006</v>
+      </c>
+      <c r="D58" s="30">
+        <f>D59+D60</f>
+        <v>4731.9598219999998</v>
+      </c>
+      <c r="E58" s="30">
+        <f>E59+E60</f>
+        <v>4282.6246919999994</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>24</v>
-      </c>
-      <c r="B59" t="s">
-        <v>24</v>
-      </c>
-      <c r="C59" s="29">
-        <f>((C55*E55)/(D55^2)-1)*100</f>
-        <v>0.80221983082513493</v>
+        <v>21</v>
+      </c>
+      <c r="C59" s="30">
+        <f>D59</f>
+        <v>2057.857317</v>
+      </c>
+      <c r="D59" s="30">
+        <v>2057.857317</v>
+      </c>
+      <c r="E59" s="30">
+        <f>D59</f>
+        <v>2057.857317</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>25</v>
-      </c>
-      <c r="B60" t="s">
-        <v>71</v>
-      </c>
-      <c r="C60" s="29">
-        <f>C58*2</f>
-        <v>21.868718815660635</v>
+        <v>22</v>
+      </c>
+      <c r="C60" s="30">
+        <v>3212.5256800000002</v>
+      </c>
+      <c r="D60" s="30">
+        <v>2674.1025049999998</v>
+      </c>
+      <c r="E60" s="30">
+        <v>2224.7673749999999</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>181</v>
+        <v>23</v>
       </c>
       <c r="B61" t="s">
-        <v>184</v>
+        <v>70</v>
       </c>
       <c r="C61" s="29">
-        <f>C60</f>
-        <v>21.868718815660635</v>
+        <f>((C58/E58)^(1/2)-1)*100</f>
+        <v>10.934359407830318</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>182</v>
+        <v>24</v>
       </c>
       <c r="B62" t="s">
-        <v>185</v>
+        <v>24</v>
       </c>
       <c r="C62" s="29">
-        <f>C58</f>
-        <v>10.934359407830318</v>
+        <f>((C58*E58)/(D58^2)-1)*100</f>
+        <v>0.80221983082513493</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>183</v>
+        <v>25</v>
       </c>
       <c r="B63" t="s">
-        <v>186</v>
+        <v>71</v>
       </c>
       <c r="C63" s="29">
-        <f>(C60-C62)/45</f>
-        <v>0.24298576461845151</v>
+        <f>C61*2</f>
+        <v>21.868718815660635</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>85</v>
+        <v>181</v>
       </c>
       <c r="B64" t="s">
-        <v>90</v>
-      </c>
-      <c r="C64" s="62">
-        <v>7.609863E-2</v>
+        <v>184</v>
+      </c>
+      <c r="C64" s="29">
+        <f>C63</f>
+        <v>21.868718815660635</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>86</v>
+        <v>182</v>
       </c>
       <c r="B65" t="s">
-        <v>89</v>
-      </c>
-      <c r="C65" s="62">
-        <v>6.7256999999999997E-2</v>
+        <v>185</v>
+      </c>
+      <c r="C65" s="29">
+        <f>C61</f>
+        <v>10.934359407830318</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>183</v>
+      </c>
+      <c r="B66" t="s">
+        <v>186</v>
+      </c>
+      <c r="C66" s="29">
+        <f>(C63-C65)/45</f>
+        <v>0.24298576461845151</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>85</v>
+      </c>
+      <c r="B67" t="s">
+        <v>90</v>
+      </c>
+      <c r="C67" s="62">
+        <v>7.609863E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>86</v>
+      </c>
+      <c r="B68" t="s">
+        <v>89</v>
+      </c>
+      <c r="C68" s="62">
+        <v>6.7256999999999997E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>87</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B69" t="s">
         <v>88</v>
       </c>
-      <c r="C66" s="62">
+      <c r="C69" s="62">
         <v>0.114567006975394</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C35">
+  <conditionalFormatting sqref="C36:C37">
     <cfRule type="expression" dxfId="9" priority="9">
       <formula>"bw57=""ADC"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
+  <conditionalFormatting sqref="C36:C37">
     <cfRule type="expression" dxfId="8" priority="10">
-      <formula>$DC$40="ADC"</formula>
+      <formula>$DC$43="ADC"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
+  <conditionalFormatting sqref="C38:C39">
     <cfRule type="expression" dxfId="7" priority="7">
       <formula>"bw57=""ADC"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
+  <conditionalFormatting sqref="C38:C39">
     <cfRule type="expression" dxfId="6" priority="8">
-      <formula>$DC$40="ADC"</formula>
+      <formula>$DC$43="ADC"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C38">
+  <conditionalFormatting sqref="C41">
     <cfRule type="expression" dxfId="5" priority="5">
       <formula>"bw57=""ADC"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C38">
+  <conditionalFormatting sqref="C41">
     <cfRule type="expression" dxfId="4" priority="6">
-      <formula>$DC$40="ADC"</formula>
+      <formula>$DC$43="ADC"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C39">
+  <conditionalFormatting sqref="C42">
     <cfRule type="expression" dxfId="3" priority="3">
       <formula>"bw57=""ADC"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C39">
+  <conditionalFormatting sqref="C42">
     <cfRule type="expression" dxfId="2" priority="4">
-      <formula>$DC$40="ADC"</formula>
+      <formula>$DC$43="ADC"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
+  <conditionalFormatting sqref="C40">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>"bw57=""ADC"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
+  <conditionalFormatting sqref="C40">
     <cfRule type="expression" dxfId="0" priority="2">
-      <formula>$DC$40="ADC"</formula>
+      <formula>$DC$43="ADC"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2780,7 +2835,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2912,32 +2967,32 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="66" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="B13" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="C13" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="66" t="s">
+        <v>265</v>
+      </c>
+      <c r="B14" t="s">
         <v>270</v>
       </c>
-      <c r="B14" t="s">
-        <v>275</v>
-      </c>
       <c r="C14" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B15" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C15" t="s">
         <v>113</v>
@@ -4347,1042 +4402,1226 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:J60"/>
+  <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.5" customWidth="1"/>
-    <col min="3" max="3" width="20.5" customWidth="1"/>
-    <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="9" max="9" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="20.5" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="10" max="10" width="20.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>43</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="F1" s="14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2022</v>
       </c>
       <c r="B2" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C2" s="16">
-        <v>-0.24</v>
-      </c>
-      <c r="D2" s="16">
-        <v>-0.24</v>
-      </c>
-      <c r="E2" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="C2" s="15">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="D2" s="15">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="E2" s="15">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="F2" s="15">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2023</v>
       </c>
       <c r="B3" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C3" s="18">
-        <v>0.11</v>
-      </c>
-      <c r="D3" s="18">
-        <v>0.11</v>
-      </c>
-      <c r="E3" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C3" s="15">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D3" s="16">
+        <v>-0.24</v>
+      </c>
+      <c r="E3" s="16">
+        <v>-0.24</v>
+      </c>
+      <c r="F3" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2024</v>
       </c>
       <c r="B4" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C4" s="18">
-        <v>0.11</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C4" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D4" s="18">
         <v>0.11</v>
       </c>
-      <c r="E4" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E4" s="18">
+        <v>0.11</v>
+      </c>
+      <c r="F4" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2025</v>
       </c>
       <c r="B5" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C5" s="18">
-        <v>0.11</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C5" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D5" s="18">
         <v>0.11</v>
       </c>
-      <c r="E5" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E5" s="18">
+        <v>0.11</v>
+      </c>
+      <c r="F5" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2026</v>
       </c>
       <c r="B6" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C6" s="19">
-        <v>0.06</v>
-      </c>
-      <c r="D6" s="19">
-        <v>0.06</v>
-      </c>
-      <c r="E6" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C6" s="15">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D6" s="18">
+        <v>0.11</v>
+      </c>
+      <c r="E6" s="18">
+        <v>0.11</v>
+      </c>
+      <c r="F6" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2027</v>
       </c>
       <c r="B7" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C7" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C7" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D7" s="19">
         <v>0.06</v>
       </c>
-      <c r="E7" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E7" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F7" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2028</v>
       </c>
       <c r="B8" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C8" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C8" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D8" s="19">
         <v>0.06</v>
       </c>
-      <c r="E8" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E8" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F8" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2029</v>
       </c>
       <c r="B9" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C9" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C9" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D9" s="19">
         <v>0.06</v>
       </c>
-      <c r="E9" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E9" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F9" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2030</v>
       </c>
       <c r="B10" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C10" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C10" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D10" s="19">
         <v>0.06</v>
       </c>
-      <c r="E10" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E10" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F10" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2031</v>
       </c>
       <c r="B11" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C11" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C11" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D11" s="19">
         <v>0.06</v>
       </c>
-      <c r="E11" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E11" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F11" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2032</v>
       </c>
       <c r="B12" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C12" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C12" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D12" s="19">
         <v>0.06</v>
       </c>
-      <c r="E12" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E12" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F12" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2033</v>
       </c>
       <c r="B13" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C13" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C13" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D13" s="19">
         <v>0.06</v>
       </c>
-      <c r="E13" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E13" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F13" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2034</v>
       </c>
       <c r="B14" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C14" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C14" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D14" s="19">
         <v>0.06</v>
       </c>
-      <c r="E14" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E14" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F14" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2035</v>
       </c>
       <c r="B15" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C15" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C15" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D15" s="19">
         <v>0.06</v>
       </c>
-      <c r="E15" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E15" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F15" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2036</v>
       </c>
       <c r="B16" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C16" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C16" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D16" s="19">
         <v>0.06</v>
       </c>
-      <c r="E16" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E16" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F16" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2037</v>
       </c>
       <c r="B17" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C17" s="19">
-        <v>0.06</v>
-      </c>
-      <c r="D17" s="18">
-        <v>-0.24</v>
-      </c>
-      <c r="E17" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C17" s="15">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D17" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="E17" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F17" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2038</v>
       </c>
       <c r="B18" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C18" s="19">
-        <v>0.06</v>
-      </c>
-      <c r="D18" s="18">
-        <v>0.11</v>
-      </c>
-      <c r="E18" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C18" s="15">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D18" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="E18" s="18">
+        <v>-0.24</v>
+      </c>
+      <c r="F18" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2039</v>
       </c>
       <c r="B19" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C19" s="19">
-        <v>0.06</v>
-      </c>
-      <c r="D19" s="18">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C19" s="15">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D19" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="E19" s="18">
         <v>0.11</v>
       </c>
-      <c r="E19" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F19" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2040</v>
       </c>
       <c r="B20" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C20" s="19">
-        <v>0.06</v>
-      </c>
-      <c r="D20" s="18">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C20" s="15">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D20" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="E20" s="18">
         <v>0.11</v>
       </c>
-      <c r="E20" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F20" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2041</v>
       </c>
       <c r="B21" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C21" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C21" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D21" s="19">
         <v>0.06</v>
       </c>
-      <c r="E21" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E21" s="18">
+        <v>0.11</v>
+      </c>
+      <c r="F21" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2042</v>
       </c>
       <c r="B22" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C22" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C22" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D22" s="19">
         <v>0.06</v>
       </c>
-      <c r="E22" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E22" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F22" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2043</v>
       </c>
       <c r="B23" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C23" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C23" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D23" s="19">
         <v>0.06</v>
       </c>
-      <c r="E23" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E23" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F23" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2044</v>
       </c>
       <c r="B24" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C24" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C24" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D24" s="19">
         <v>0.06</v>
       </c>
-      <c r="E24" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E24" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F24" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2045</v>
       </c>
       <c r="B25" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C25" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C25" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D25" s="19">
         <v>0.06</v>
       </c>
-      <c r="E25" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E25" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F25" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2046</v>
       </c>
       <c r="B26" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C26" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C26" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D26" s="19">
         <v>0.06</v>
       </c>
-      <c r="E26" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E26" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F26" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2047</v>
       </c>
       <c r="B27" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C27" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C27" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D27" s="19">
         <v>0.06</v>
       </c>
-      <c r="E27" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E27" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F27" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2048</v>
       </c>
       <c r="B28" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C28" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C28" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D28" s="19">
         <v>0.06</v>
       </c>
-      <c r="E28" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E28" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F28" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2049</v>
       </c>
       <c r="B29" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C29" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C29" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D29" s="19">
         <v>0.06</v>
       </c>
-      <c r="E29" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E29" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F29" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2050</v>
       </c>
       <c r="B30" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C30" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C30" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D30" s="19">
         <v>0.06</v>
       </c>
-      <c r="E30" s="17">
-        <v>0.06</v>
-      </c>
-      <c r="I30" s="71"/>
-      <c r="J30" s="27"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E30" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F30" s="17">
+        <v>0.06</v>
+      </c>
+      <c r="J30" s="71"/>
+      <c r="K30" s="27"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2051</v>
       </c>
       <c r="B31" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C31" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C31" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D31" s="19">
         <v>0.06</v>
       </c>
-      <c r="E31" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E31" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F31" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2052</v>
       </c>
       <c r="B32" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C32" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C32" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D32" s="19">
         <v>0.06</v>
       </c>
-      <c r="E32" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E32" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F32" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2053</v>
       </c>
       <c r="B33" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C33" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C33" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D33" s="19">
         <v>0.06</v>
       </c>
-      <c r="E33" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E33" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F33" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>2054</v>
       </c>
       <c r="B34" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C34" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C34" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D34" s="19">
         <v>0.06</v>
       </c>
-      <c r="E34" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E34" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F34" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2055</v>
       </c>
       <c r="B35" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C35" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C35" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D35" s="19">
         <v>0.06</v>
       </c>
-      <c r="E35" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E35" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F35" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>2056</v>
       </c>
       <c r="B36" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C36" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C36" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D36" s="19">
         <v>0.06</v>
       </c>
-      <c r="E36" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E36" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F36" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>2057</v>
       </c>
       <c r="B37" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C37" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C37" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D37" s="19">
         <v>0.06</v>
       </c>
-      <c r="E37" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E37" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F37" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>2058</v>
       </c>
       <c r="B38" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C38" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C38" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D38" s="19">
         <v>0.06</v>
       </c>
-      <c r="E38" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E38" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F38" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>2059</v>
       </c>
       <c r="B39" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C39" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C39" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D39" s="19">
         <v>0.06</v>
       </c>
-      <c r="E39" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E39" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F39" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2060</v>
       </c>
       <c r="B40" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C40" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C40" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D40" s="19">
         <v>0.06</v>
       </c>
-      <c r="E40" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E40" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F40" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>2061</v>
       </c>
       <c r="B41" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C41" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C41" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D41" s="19">
         <v>0.06</v>
       </c>
-      <c r="E41" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E41" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F41" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>2062</v>
       </c>
       <c r="B42" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C42" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C42" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D42" s="19">
         <v>0.06</v>
       </c>
-      <c r="E42" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E42" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F42" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>2063</v>
       </c>
       <c r="B43" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C43" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C43" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D43" s="19">
         <v>0.06</v>
       </c>
-      <c r="E43" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E43" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F43" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>2064</v>
       </c>
       <c r="B44" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C44" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C44" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D44" s="19">
         <v>0.06</v>
       </c>
-      <c r="E44" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E44" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F44" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>2065</v>
       </c>
       <c r="B45" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C45" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C45" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D45" s="19">
         <v>0.06</v>
       </c>
-      <c r="E45" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E45" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F45" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>2066</v>
       </c>
       <c r="B46" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C46" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C46" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D46" s="19">
         <v>0.06</v>
       </c>
-      <c r="E46" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E46" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F46" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>2067</v>
       </c>
       <c r="B47" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C47" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C47" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D47" s="19">
         <v>0.06</v>
       </c>
-      <c r="E47" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E47" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F47" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>2068</v>
       </c>
       <c r="B48" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C48" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C48" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D48" s="19">
         <v>0.06</v>
       </c>
-      <c r="E48" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E48" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F48" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>2069</v>
       </c>
       <c r="B49" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C49" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C49" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D49" s="19">
         <v>0.06</v>
       </c>
-      <c r="E49" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E49" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F49" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>2070</v>
       </c>
       <c r="B50" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C50" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C50" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D50" s="19">
         <v>0.06</v>
       </c>
-      <c r="E50" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E50" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F50" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>2071</v>
       </c>
       <c r="B51" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C51" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C51" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D51" s="19">
         <v>0.06</v>
       </c>
-      <c r="E51" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E51" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F51" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>2072</v>
       </c>
       <c r="B52" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C52" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C52" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D52" s="19">
         <v>0.06</v>
       </c>
-      <c r="E52" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E52" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F52" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>2073</v>
       </c>
       <c r="B53" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C53" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C53" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D53" s="19">
         <v>0.06</v>
       </c>
-      <c r="E53" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E53" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F53" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>2074</v>
       </c>
       <c r="B54" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C54" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C54" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D54" s="19">
         <v>0.06</v>
       </c>
-      <c r="E54" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E54" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F54" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>2075</v>
       </c>
       <c r="B55" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C55" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C55" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D55" s="19">
         <v>0.06</v>
       </c>
-      <c r="E55" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E55" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F55" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>2076</v>
       </c>
       <c r="B56" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C56" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C56" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D56" s="19">
         <v>0.06</v>
       </c>
-      <c r="E56" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E56" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F56" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>2077</v>
       </c>
       <c r="B57" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C57" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C57" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D57" s="19">
         <v>0.06</v>
       </c>
-      <c r="E57" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E57" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F57" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>2078</v>
       </c>
       <c r="B58" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C58" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C58" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D58" s="19">
         <v>0.06</v>
       </c>
-      <c r="E58" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E58" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F58" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>2079</v>
       </c>
       <c r="B59" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C59" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C59" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D59" s="19">
         <v>0.06</v>
       </c>
-      <c r="E59" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E59" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F59" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>2080</v>
       </c>
       <c r="B60" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C60" s="19">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C60" s="15">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D60" s="19">
         <v>0.06</v>
       </c>
-      <c r="E60" s="17">
-        <v>0.06</v>
-      </c>
+      <c r="E60" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="F60" s="17">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D61" s="78"/>
+      <c r="E61" s="78"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5393,7 +5632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:DA13"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="111" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="AI1" zoomScale="111" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="AP7" sqref="AP7"/>
     </sheetView>
   </sheetViews>
@@ -5509,7 +5748,7 @@
         <v>201</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>202</v>
@@ -5587,7 +5826,7 @@
         <v>79</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="AE1" s="1" t="s">
         <v>123</v>
@@ -5599,7 +5838,7 @@
         <v>80</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="AI1" s="1" t="s">
         <v>125</v>
@@ -5644,22 +5883,22 @@
         <v>135</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="AX1" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="BA1" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="AY1" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>260</v>
-      </c>
       <c r="BB1" s="4" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="BC1" s="4" t="s">
         <v>136</v>
@@ -5668,16 +5907,16 @@
         <v>137</v>
       </c>
       <c r="BE1" s="4" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="BF1" s="4" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="BG1" s="1" t="s">
         <v>206</v>
       </c>
       <c r="BH1" s="1" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="BI1" s="1" t="s">
         <v>138</v>
@@ -5692,7 +5931,7 @@
         <v>141</v>
       </c>
       <c r="BM1" s="1" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="BN1" s="1" t="s">
         <v>187</v>
@@ -5725,19 +5964,19 @@
         <v>143</v>
       </c>
       <c r="BX1" s="1" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="BY1" s="3" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="BZ1" s="3" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="CA1" s="3" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="CB1" s="3" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="CC1" s="5" t="s">
         <v>200</v>
@@ -5752,7 +5991,7 @@
         <v>196</v>
       </c>
       <c r="CG1" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="CH1" t="s">
         <v>144</v>
@@ -5764,7 +6003,7 @@
         <v>146</v>
       </c>
       <c r="CK1" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="CL1" t="s">
         <v>147</v>
@@ -5776,10 +6015,10 @@
         <v>149</v>
       </c>
       <c r="CO1" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="CP1" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="CQ1" t="s">
         <v>150</v>
@@ -5794,7 +6033,7 @@
         <v>153</v>
       </c>
       <c r="CU1" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="CV1" t="s">
         <v>154</v>
@@ -5806,10 +6045,10 @@
         <v>156</v>
       </c>
       <c r="CY1" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="CZ1" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2" spans="1:105" s="24" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>